<commit_message>
Reportes de Facilitacion (Excel)
</commit_message>
<xml_diff>
--- a/RegionalFF/Content/Archivos/Plantilla/Plantilla.xlsx
+++ b/RegionalFF/Content/Archivos/Plantilla/Plantilla.xlsx
@@ -23,15 +23,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t xml:space="preserve">                                                                                            </t>
-  </si>
-  <si>
-    <t>"Cabecera del Puente Internacional "San Roque González de Santa Cruz"</t>
-  </si>
-  <si>
-    <t>Encarnación - Paraguay</t>
   </si>
   <si>
     <t>Fecha</t>
@@ -285,9 +279,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>156142</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>7824</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1571625" cy="657225"/>
     <xdr:pic>
@@ -305,8 +299,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
+          <a:off x="156142" y="330994"/>
+          <a:ext cx="1571625" cy="657225"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -318,9 +312,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
+      <xdr:colOff>156142</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>45584</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1028700" cy="676275"/>
     <xdr:pic>
@@ -338,8 +332,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
+          <a:off x="6628039" y="368754"/>
+          <a:ext cx="1028700" cy="676275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -351,11 +345,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
+      <xdr:colOff>697366</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>153080</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1466850" cy="752475"/>
+    <xdr:ext cx="1466850" cy="711654"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="4" name="0 Imagen"/>
@@ -371,8 +365,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
+          <a:off x="2415268" y="314665"/>
+          <a:ext cx="1466850" cy="711654"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -384,11 +378,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
+      <xdr:colOff>263637</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>152159</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1085850" cy="923925"/>
+    <xdr:ext cx="954201" cy="811908"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="5" name="5 Imagen" descr="C:\Users\dgranada\Desktop\logo dmt 2016.jpg"/>
@@ -404,8 +398,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
+          <a:off x="8461941" y="313744"/>
+          <a:ext cx="954201" cy="811908"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -414,6 +408,44 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>510270</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>17010</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1156608</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>195604</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4932591" y="340180"/>
+          <a:ext cx="646338" cy="663348"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -707,7 +739,7 @@
   <dimension ref="A1:P593"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="12.75" customHeight="1"/>
@@ -827,9 +859,7 @@
       <c r="M7" s="22"/>
     </row>
     <row r="8" spans="1:16" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A8" s="39" t="s">
-        <v>1</v>
-      </c>
+      <c r="A8" s="39"/>
       <c r="B8" s="39"/>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
@@ -846,9 +876,7 @@
       <c r="O8" s="6"/>
     </row>
     <row r="9" spans="1:16" s="3" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A9" s="40" t="s">
-        <v>2</v>
-      </c>
+      <c r="A9" s="40"/>
       <c r="B9" s="40"/>
       <c r="C9" s="40"/>
       <c r="D9" s="40"/>
@@ -865,22 +893,22 @@
     </row>
     <row r="10" spans="1:16" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A10" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="D10" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="E10" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="F10" s="25" t="s">
         <v>6</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="25" t="s">
-        <v>8</v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="15"/>
@@ -899,7 +927,7 @@
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
       <c r="E11" s="25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F11" s="25"/>
       <c r="G11" s="19"/>

</xml_diff>